<commit_message>
update to 24min duration
</commit_message>
<xml_diff>
--- a/res/trials.xlsx
+++ b/res/trials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rima-mariarahal/science/keeplooking/keeplooking/res/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rima-mariarahal/science/globalbluegreen/globalbluegreen/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8177E5A2-D22E-C64E-AD1A-B56ED9E0EA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CA84EC-79F0-0446-B815-181A319A4D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="2340" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{46A3392B-8735-774F-B60D-1E4EA857EEDA}"/>
   </bookViews>
@@ -27,14 +27,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -64,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
   <si>
     <t>s1</t>
   </si>
@@ -115,6 +107,9 @@
   </si>
   <si>
     <t>finalitemnr</t>
+  </si>
+  <si>
+    <t>left_prosocial</t>
   </si>
 </sst>
 </file>
@@ -6453,7 +6448,7 @@
         <v>1</v>
       </c>
       <c r="X66">
-        <f t="shared" ref="X66:X97" si="34">IF(AND(V66&gt;0,W66&lt;0),1,0)</f>
+        <f t="shared" ref="X66:X81" si="34">IF(AND(V66&gt;0,W66&lt;0),1,0)</f>
         <v>0</v>
       </c>
       <c r="Y66">
@@ -6461,7 +6456,7 @@
         <v>1</v>
       </c>
       <c r="Z66" t="b">
-        <f t="shared" ref="Z66:Z97" si="36">(X66+Y66)&gt;0</f>
+        <f t="shared" ref="Z66:Z81" si="36">(X66+Y66)&gt;0</f>
         <v>1</v>
       </c>
     </row>
@@ -7854,7 +7849,7 @@
       </c>
       <c r="B1">
         <f t="shared" ref="B1:B32" ca="1" si="0">RANDBETWEEN(1,10000)</f>
-        <v>2328</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -7863,7 +7858,7 @@
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>4323</v>
+        <v>2328</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -7872,7 +7867,7 @@
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>9724</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -7881,7 +7876,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>7674</v>
+        <v>2918</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -7890,7 +7885,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>3988</v>
+        <v>4307</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -7899,7 +7894,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>5283</v>
+        <v>2477</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -7908,7 +7903,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>6914</v>
+        <v>7193</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -7917,7 +7912,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>1270</v>
+        <v>7204</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -7926,7 +7921,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>4205</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -7935,7 +7930,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>3543</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -7944,7 +7939,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>7518</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -7953,7 +7948,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>2495</v>
+        <v>5768</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -7962,7 +7957,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>3248</v>
+        <v>6748</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -7971,7 +7966,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>7025</v>
+        <v>4474</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -7980,7 +7975,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>179</v>
+        <v>7842</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -7989,7 +7984,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>659</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -7998,7 +7993,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>9191</v>
+        <v>855</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -8007,7 +8002,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>723</v>
+        <v>9503</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -8016,7 +8011,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>2053</v>
+        <v>988</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -8025,7 +8020,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>8311</v>
+        <v>4774</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -8034,7 +8029,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>3001</v>
+        <v>5803</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -8043,7 +8038,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>7029</v>
+        <v>4302</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -8052,7 +8047,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>8199</v>
+        <v>487</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -8061,7 +8056,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>7272</v>
+        <v>9177</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -8070,7 +8065,7 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>3093</v>
+        <v>8192</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -8079,7 +8074,7 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>8463</v>
+        <v>4032</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -8088,7 +8083,7 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>5393</v>
+        <v>3699</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -8097,7 +8092,7 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>2469</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -8106,7 +8101,7 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>4033</v>
+        <v>3401</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -8115,7 +8110,7 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>2194</v>
+        <v>591</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -8124,7 +8119,7 @@
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>4366</v>
+        <v>3360</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -8133,7 +8128,7 @@
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>6995</v>
+        <v>7886</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -8142,7 +8137,7 @@
       </c>
       <c r="B33">
         <f t="shared" ref="B33:B64" ca="1" si="1">RANDBETWEEN(1,10000)</f>
-        <v>2875</v>
+        <v>9134</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -8151,7 +8146,7 @@
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="1"/>
-        <v>8926</v>
+        <v>226</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -8160,7 +8155,7 @@
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="1"/>
-        <v>5865</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -8169,7 +8164,7 @@
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="1"/>
-        <v>3709</v>
+        <v>3722</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -8178,7 +8173,7 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="1"/>
-        <v>1878</v>
+        <v>7828</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -8187,7 +8182,7 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="1"/>
-        <v>1996</v>
+        <v>3834</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -8196,7 +8191,7 @@
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="1"/>
-        <v>164</v>
+        <v>8436</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -8205,7 +8200,7 @@
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="1"/>
-        <v>2489</v>
+        <v>5591</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -8214,7 +8209,7 @@
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="1"/>
-        <v>7507</v>
+        <v>9688</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -8223,7 +8218,7 @@
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="1"/>
-        <v>5656</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -8232,7 +8227,7 @@
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="1"/>
-        <v>1746</v>
+        <v>9380</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -8241,7 +8236,7 @@
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="1"/>
-        <v>4518</v>
+        <v>5248</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -8250,7 +8245,7 @@
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="1"/>
-        <v>1127</v>
+        <v>5937</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -8259,7 +8254,7 @@
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="1"/>
-        <v>1472</v>
+        <v>9662</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -8268,7 +8263,7 @@
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="1"/>
-        <v>2698</v>
+        <v>8460</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -8277,7 +8272,7 @@
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="1"/>
-        <v>8995</v>
+        <v>4576</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -8286,7 +8281,7 @@
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="1"/>
-        <v>6503</v>
+        <v>9352</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -8295,7 +8290,7 @@
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="1"/>
-        <v>3669</v>
+        <v>5190</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -8304,7 +8299,7 @@
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="1"/>
-        <v>6251</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -8313,7 +8308,7 @@
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="1"/>
-        <v>9947</v>
+        <v>3916</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -8322,7 +8317,7 @@
       </c>
       <c r="B53">
         <f t="shared" ca="1" si="1"/>
-        <v>2936</v>
+        <v>6112</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -8331,7 +8326,7 @@
       </c>
       <c r="B54">
         <f t="shared" ca="1" si="1"/>
-        <v>1285</v>
+        <v>5406</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -8340,7 +8335,7 @@
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="1"/>
-        <v>8095</v>
+        <v>3975</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -8349,7 +8344,7 @@
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="1"/>
-        <v>6124</v>
+        <v>336</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -8358,7 +8353,7 @@
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="1"/>
-        <v>5392</v>
+        <v>2675</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -8367,7 +8362,7 @@
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="1"/>
-        <v>7669</v>
+        <v>4012</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -8376,7 +8371,7 @@
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="1"/>
-        <v>6575</v>
+        <v>8188</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -8385,7 +8380,7 @@
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="1"/>
-        <v>3404</v>
+        <v>737</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -8394,7 +8389,7 @@
       </c>
       <c r="B61">
         <f t="shared" ca="1" si="1"/>
-        <v>894</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -8403,7 +8398,7 @@
       </c>
       <c r="B62">
         <f t="shared" ca="1" si="1"/>
-        <v>6279</v>
+        <v>612</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -8412,7 +8407,7 @@
       </c>
       <c r="B63">
         <f t="shared" ca="1" si="1"/>
-        <v>52</v>
+        <v>7915</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -8421,7 +8416,7 @@
       </c>
       <c r="B64">
         <f t="shared" ca="1" si="1"/>
-        <v>9337</v>
+        <v>7772</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -8430,7 +8425,7 @@
       </c>
       <c r="B65">
         <f t="shared" ref="B65:B80" ca="1" si="2">RANDBETWEEN(1,10000)</f>
-        <v>7015</v>
+        <v>3444</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -8439,7 +8434,7 @@
       </c>
       <c r="B66">
         <f t="shared" ca="1" si="2"/>
-        <v>6296</v>
+        <v>8117</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -8448,7 +8443,7 @@
       </c>
       <c r="B67">
         <f t="shared" ca="1" si="2"/>
-        <v>9524</v>
+        <v>6913</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -8457,7 +8452,7 @@
       </c>
       <c r="B68">
         <f t="shared" ca="1" si="2"/>
-        <v>3829</v>
+        <v>5599</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -8466,7 +8461,7 @@
       </c>
       <c r="B69">
         <f t="shared" ca="1" si="2"/>
-        <v>7209</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -8475,7 +8470,7 @@
       </c>
       <c r="B70">
         <f t="shared" ca="1" si="2"/>
-        <v>8640</v>
+        <v>5803</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
@@ -8484,7 +8479,7 @@
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="2"/>
-        <v>7575</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -8493,7 +8488,7 @@
       </c>
       <c r="B72">
         <f t="shared" ca="1" si="2"/>
-        <v>1661</v>
+        <v>7008</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -8502,7 +8497,7 @@
       </c>
       <c r="B73">
         <f t="shared" ca="1" si="2"/>
-        <v>9331</v>
+        <v>6116</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -8511,7 +8506,7 @@
       </c>
       <c r="B74">
         <f t="shared" ca="1" si="2"/>
-        <v>9277</v>
+        <v>4514</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -8520,7 +8515,7 @@
       </c>
       <c r="B75">
         <f t="shared" ca="1" si="2"/>
-        <v>9688</v>
+        <v>296</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -8529,7 +8524,7 @@
       </c>
       <c r="B76">
         <f t="shared" ca="1" si="2"/>
-        <v>9296</v>
+        <v>9359</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -8538,7 +8533,7 @@
       </c>
       <c r="B77">
         <f t="shared" ca="1" si="2"/>
-        <v>8206</v>
+        <v>99</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -8547,7 +8542,7 @@
       </c>
       <c r="B78">
         <f t="shared" ca="1" si="2"/>
-        <v>4374</v>
+        <v>8956</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
@@ -8556,7 +8551,7 @@
       </c>
       <c r="B79">
         <f t="shared" ca="1" si="2"/>
-        <v>6885</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -8565,7 +8560,7 @@
       </c>
       <c r="B80">
         <f t="shared" ca="1" si="2"/>
-        <v>1763</v>
+        <v>5966</v>
       </c>
     </row>
   </sheetData>
@@ -8580,15 +8575,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C6D6DE-18C2-5D4D-BAF0-7F3FEB66671F}">
-  <dimension ref="A1:Q61"/>
+  <dimension ref="A1:R61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -8640,8 +8635,11 @@
       <c r="Q1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8693,8 +8691,12 @@
       <c r="Q2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R2">
+        <f>IF(C2&gt;E2,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -8746,8 +8748,12 @@
       <c r="Q3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R3">
+        <f t="shared" ref="R3:R61" si="0">IF(C3&gt;E3,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -8799,8 +8805,12 @@
       <c r="Q4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -8852,8 +8862,12 @@
       <c r="Q5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -8905,8 +8919,12 @@
       <c r="Q6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -8958,8 +8976,12 @@
       <c r="Q7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -9011,8 +9033,12 @@
       <c r="Q8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -9064,8 +9090,12 @@
       <c r="Q9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -9117,8 +9147,12 @@
       <c r="Q10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -9170,8 +9204,12 @@
       <c r="Q11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -9223,8 +9261,12 @@
       <c r="Q12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -9276,8 +9318,12 @@
       <c r="Q13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -9329,8 +9375,12 @@
       <c r="Q14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -9382,8 +9432,12 @@
       <c r="Q15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -9435,8 +9489,12 @@
       <c r="Q16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -9488,8 +9546,12 @@
       <c r="Q17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -9541,8 +9603,12 @@
       <c r="Q18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -9594,8 +9660,12 @@
       <c r="Q19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -9647,8 +9717,12 @@
       <c r="Q20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -9700,8 +9774,12 @@
       <c r="Q21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -9753,8 +9831,12 @@
       <c r="Q22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -9806,8 +9888,12 @@
       <c r="Q23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -9859,8 +9945,12 @@
       <c r="Q24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -9912,8 +10002,12 @@
       <c r="Q25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -9965,8 +10059,12 @@
       <c r="Q26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -10018,8 +10116,12 @@
       <c r="Q27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -10071,8 +10173,12 @@
       <c r="Q28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -10124,8 +10230,12 @@
       <c r="Q29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -10177,8 +10287,12 @@
       <c r="Q30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -10230,8 +10344,12 @@
       <c r="Q31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -10283,8 +10401,12 @@
       <c r="Q32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -10336,8 +10458,12 @@
       <c r="Q33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -10389,8 +10515,12 @@
       <c r="Q34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -10442,8 +10572,12 @@
       <c r="Q35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -10495,8 +10629,12 @@
       <c r="Q36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -10548,8 +10686,12 @@
       <c r="Q37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -10601,8 +10743,12 @@
       <c r="Q38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -10654,8 +10800,12 @@
       <c r="Q39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -10707,8 +10857,12 @@
       <c r="Q40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -10760,8 +10914,12 @@
       <c r="Q41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -10813,8 +10971,12 @@
       <c r="Q42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -10866,8 +11028,12 @@
       <c r="Q43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -10919,8 +11085,12 @@
       <c r="Q44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -10972,8 +11142,12 @@
       <c r="Q45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -11025,8 +11199,12 @@
       <c r="Q46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R46">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -11078,8 +11256,12 @@
       <c r="Q47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R47">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -11131,8 +11313,12 @@
       <c r="Q48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -11184,8 +11370,12 @@
       <c r="Q49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -11237,8 +11427,12 @@
       <c r="Q50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -11290,8 +11484,12 @@
       <c r="Q51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -11343,8 +11541,12 @@
       <c r="Q52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -11396,8 +11598,12 @@
       <c r="Q53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -11449,8 +11655,12 @@
       <c r="Q54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R54">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -11502,8 +11712,12 @@
       <c r="Q55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R55">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -11555,8 +11769,12 @@
       <c r="Q56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R56">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -11608,8 +11826,12 @@
       <c r="Q57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -11661,8 +11883,12 @@
       <c r="Q58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R58">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -11714,8 +11940,12 @@
       <c r="Q59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R59">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -11767,8 +11997,12 @@
       <c r="Q60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R60">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -11819,6 +12053,10 @@
       </c>
       <c r="Q61">
         <v>1</v>
+      </c>
+      <c r="R61">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>